<commit_message>
Añadidos ficheros de prueba, actualizado función de petición de vacunas para añadir el ID utilizado en get_vaccine_date. Añadidos casos de prueba de la segunda función al Excel.
</commit_message>
<xml_diff>
--- a/docs/Casos de prueba.xlsx
+++ b/docs/Casos de prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\G80.2022.T10.EG3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB906399-5005-4149-8415-9BF3C535D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F03CA4F-A75E-485C-B479-97527D3B22E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="312">
   <si>
     <t>I/O</t>
   </si>
@@ -76,12 +76,6 @@
     <t>VALID</t>
   </si>
   <si>
-    <t>12345678Z</t>
-  </si>
-  <si>
-    <t>&lt;valid hash for these values&gt;</t>
-  </si>
-  <si>
     <t>INVALID</t>
   </si>
   <si>
@@ -100,12 +94,6 @@
     <t>FILE CONTENT</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>Initial brace deleted</t>
-  </si>
-  <si>
     <t>PATH</t>
   </si>
   <si>
@@ -113,9 +101,6 @@
   </si>
   <si>
     <t>1_3_5_6_8_10</t>
-  </si>
-  <si>
-    <t>id_of_your_testcase</t>
   </si>
   <si>
     <t>patient_id</t>
@@ -505,6 +490,528 @@
   <si>
     <t>Teléfono demasiado corto</t>
   </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Ambos</t>
+  </si>
+  <si>
+    <t>test1_get_vaccine_date_ok</t>
+  </si>
+  <si>
+    <t>Caso válido</t>
+  </si>
+  <si>
+    <t>test_get_vaccine_date_ok.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>Código válido</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>DELETION</t>
+  </si>
+  <si>
+    <t>test_vacio</t>
+  </si>
+  <si>
+    <t>Fichero vacío (nodo 1 eliminado)</t>
+  </si>
+  <si>
+    <t>test_vacio.json</t>
+  </si>
+  <si>
+    <t>(vacío)</t>
+  </si>
+  <si>
+    <t>DUPLICATION</t>
+  </si>
+  <si>
+    <t>test_doble</t>
+  </si>
+  <si>
+    <t>Fichero duplicado</t>
+  </si>
+  <si>
+    <t>test_doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>NT, T</t>
+  </si>
+  <si>
+    <t>test_sinprimerbracket</t>
+  </si>
+  <si>
+    <t>Elimino el primer corchete</t>
+  </si>
+  <si>
+    <t>test_sinprimercorchete.json</t>
+  </si>
+  <si>
+    <t>"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>NT,T</t>
+  </si>
+  <si>
+    <t>test_primerbracketdoble</t>
+  </si>
+  <si>
+    <t>Duplico primero corchete</t>
+  </si>
+  <si>
+    <t>test_primerbracketdoble.json</t>
+  </si>
+  <si>
+    <t>{{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_solocorchetes</t>
+  </si>
+  <si>
+    <t>Elimino todo menos corchetes</t>
+  </si>
+  <si>
+    <t>test_solocorchetes.json</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>test_datosdobles</t>
+  </si>
+  <si>
+    <t>Los datos se repiten</t>
+  </si>
+  <si>
+    <t>test_datosdobles.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921""PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sinsegundobracket</t>
+  </si>
+  <si>
+    <t>Falta el segundo corchete</t>
+  </si>
+  <si>
+    <t>test_sinsegundobracket.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"</t>
+  </si>
+  <si>
+    <t>nt, t</t>
+  </si>
+  <si>
+    <t>test_segundobracketdoble</t>
+  </si>
+  <si>
+    <t>El segundo bracket está repetido</t>
+  </si>
+  <si>
+    <t>test_segundobracketdoble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}}</t>
+  </si>
+  <si>
+    <t>test_primercampodoble</t>
+  </si>
+  <si>
+    <t>El primer campo está duplicado</t>
+  </si>
+  <si>
+    <t>test_primercampodoble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93""PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sinprimercampo</t>
+  </si>
+  <si>
+    <t>Falta el primer campo</t>
+  </si>
+  <si>
+    <t>test_sinprimercampo.json</t>
+  </si>
+  <si>
+    <t>{,"ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sincoma</t>
+  </si>
+  <si>
+    <t>Falta la coma</t>
+  </si>
+  <si>
+    <t>test_sincoma.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93""ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_comadoble</t>
+  </si>
+  <si>
+    <t>Coma doble</t>
+  </si>
+  <si>
+    <t>test_comadoble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93",,"ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_segundocampodoble</t>
+  </si>
+  <si>
+    <t>Segundo campo doble</t>
+  </si>
+  <si>
+    <t>test_segundocampodoble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921""ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sinsegundocampo</t>
+  </si>
+  <si>
+    <t>Sin segundo campo</t>
+  </si>
+  <si>
+    <t>test_sinsegundocampo.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93",}</t>
+  </si>
+  <si>
+    <t>test_primeraetiquetadoble</t>
+  </si>
+  <si>
+    <t>Etiqueta 1 duplicada</t>
+  </si>
+  <si>
+    <t>test_primeraetiquetadoble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID""PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sinprimeraetiqueta</t>
+  </si>
+  <si>
+    <t>Etiqueta 1 borrada</t>
+  </si>
+  <si>
+    <t>test_sinprimeraetiqueta.json</t>
+  </si>
+  <si>
+    <t>{:"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>11, 20</t>
+  </si>
+  <si>
+    <t>test_sinigualdad1</t>
+  </si>
+  <si>
+    <t>Primer ":" borrado</t>
+  </si>
+  <si>
+    <t>test_sinigualdad1.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID""1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_igualdad1doble</t>
+  </si>
+  <si>
+    <t>Primer ":" duplicado</t>
+  </si>
+  <si>
+    <t>test_igualdad1doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID"::"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_dato1doble</t>
+  </si>
+  <si>
+    <t>Primer dato duplicado</t>
+  </si>
+  <si>
+    <t>test_dato1doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93""1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sindato1</t>
+  </si>
+  <si>
+    <t>Primer dato borrado</t>
+  </si>
+  <si>
+    <t>test_sindato1.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":,"ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_segundatiquetadoble</t>
+  </si>
+  <si>
+    <t>Etiqueta 2 duplicada</t>
+  </si>
+  <si>
+    <t>test_segundaetiquetadoble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber""ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sinsegundaetiqueta</t>
+  </si>
+  <si>
+    <t>Etiqueta 2 borrada</t>
+  </si>
+  <si>
+    <t>test_sinsegundaetiqueta.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93",: "923412921"}</t>
+  </si>
+  <si>
+    <t>test_igualdad2doble</t>
+  </si>
+  <si>
+    <t>Igualdad dos doble</t>
+  </si>
+  <si>
+    <t>test_igualdad2doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":: "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sinigualdad2</t>
+  </si>
+  <si>
+    <t>Igualdad dos eliminada</t>
+  </si>
+  <si>
+    <t>test_sinigualdad2.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber""923412921"}</t>
+  </si>
+  <si>
+    <t>test_dato2doble</t>
+  </si>
+  <si>
+    <t>Dato 2 duplicado</t>
+  </si>
+  <si>
+    <t>test_dato2doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921" "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sindato2</t>
+  </si>
+  <si>
+    <t>Dato 2 eliminado</t>
+  </si>
+  <si>
+    <t>test_sindato2.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":}</t>
+  </si>
+  <si>
+    <t>test_sincomilla1</t>
+  </si>
+  <si>
+    <t>Primeras comillas eliminadas</t>
+  </si>
+  <si>
+    <t>test_sincomilla1.json</t>
+  </si>
+  <si>
+    <t>{""PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla1doble</t>
+  </si>
+  <si>
+    <t>Primeras comillas duplicadas</t>
+  </si>
+  <si>
+    <t>test_comilla1doble.json</t>
+  </si>
+  <si>
+    <t>18, 32</t>
+  </si>
+  <si>
+    <t>DUPLICATION / MODIFICATION</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta1doble</t>
+  </si>
+  <si>
+    <t>Primer valor de etiqueta doble</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta1doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemIDPatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>No se elimina ya que sería una modificación, que ya está incluida aquí</t>
+  </si>
+  <si>
+    <t>19, 33</t>
+  </si>
+  <si>
+    <t>test_comilla2doble</t>
+  </si>
+  <si>
+    <t>Segundas comillas duplicadas</t>
+  </si>
+  <si>
+    <t>test_comilla2doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID"":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sincomilla2</t>
+  </si>
+  <si>
+    <t>Segundas comillas borradas</t>
+  </si>
+  <si>
+    <t>test_sincomilla2.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID:"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>21, 34</t>
+  </si>
+  <si>
+    <t>test_comilla3doble</t>
+  </si>
+  <si>
+    <t>Terceras comillas dobles</t>
+  </si>
+  <si>
+    <t>test_comilla3doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":""1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sincomilla3</t>
+  </si>
+  <si>
+    <t>Sin terceras comillas</t>
+  </si>
+  <si>
+    <t>test_sincomilla3.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>23, 36</t>
+  </si>
+  <si>
+    <t>test_comilla4doble</t>
+  </si>
+  <si>
+    <t>Cuarta comilla duplicada</t>
+  </si>
+  <si>
+    <t>test_comilla4doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93"","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_sincomilla4</t>
+  </si>
+  <si>
+    <t>Cuarta comilla eliminada</t>
+  </si>
+  <si>
+    <t>test_sincomilla4.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93,"ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>DUPLICATION/MODIFICATION</t>
+  </si>
+  <si>
+    <t>test_valordato1duplicado</t>
+  </si>
+  <si>
+    <t>Valor dato1 duplicado y modificado</t>
+  </si>
+  <si>
+    <t>test_valordato1duplicado.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d931c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>25, 38</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta2doble</t>
+  </si>
+  <si>
+    <t>Valor etiqueta 2 duplicado y modificado por tanto</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta2doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumberContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>29, 41</t>
+  </si>
+  <si>
+    <t>test_valordato2doble</t>
+  </si>
+  <si>
+    <t>Valor dato 2 duplicado y por tanto modificado</t>
+  </si>
+  <si>
+    <t>test_valordato2doble.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921923412921"}</t>
+  </si>
 </sst>
 </file>
 
@@ -520,6 +1027,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -621,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -651,11 +1159,37 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -695,28 +1229,6 @@
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
       </font>
     </dxf>
     <dxf>
@@ -869,39 +1381,39 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="FIELD"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="VALID/INVALID"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="ID TEST"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DESCRIPTION" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="DESCRIPTION" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="patient_id "/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="registration_type"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="name_surname"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="phone_number"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="age"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="EXPECTED RESULT" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="OBSERVATIONS" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="EXPECTED RESULT" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="OBSERVATIONS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="GE3 2021 F1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A1:J43" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C943CFE-479E-4F17-9794-3B0A241BDC37}" name="Table_32" displayName="Table_32" ref="A1:J43" headerRowDxfId="0">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="#"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="NODE"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="TERMINAL  (T) / NO TERMINAL (NT)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="ID TEST"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="DESCRIPTION"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="FILE PATH"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="FILE CONTENT"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="EXPECTED RESULT"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="OBSERVATIONS"/>
+    <tableColumn id="1" xr3:uid="{93B13E22-E985-4930-A193-EA9B9D4B2027}" name="#"/>
+    <tableColumn id="2" xr3:uid="{BE1F42EC-89F3-4ED3-A311-BA3B85140EF4}" name="NODE"/>
+    <tableColumn id="3" xr3:uid="{BBE1E901-BCD1-4253-99F2-8AA9F6201F80}" name="TERMINAL  (T) / NO TERMINAL (NT)"/>
+    <tableColumn id="4" xr3:uid="{466D5E0E-10A6-4079-87D9-E2839D0DC345}" name="TYPE (DUPLICATION / DELETION / MODIFICATION / VALID)"/>
+    <tableColumn id="5" xr3:uid="{C749B9BD-54F7-43A3-BF7A-DBB1809A505E}" name="ID TEST"/>
+    <tableColumn id="6" xr3:uid="{B1A1B8DC-3D3C-4E85-99BD-9456D75FC99D}" name="DESCRIPTION"/>
+    <tableColumn id="7" xr3:uid="{2453D50B-47F4-4948-B608-E0408654E0CE}" name="FILE PATH"/>
+    <tableColumn id="8" xr3:uid="{3A33E620-9652-4A0F-AC53-983688774C0B}" name="FILE CONTENT"/>
+    <tableColumn id="9" xr3:uid="{FAC4C052-5274-466B-A80D-15E562E05CA8}" name="EXPECTED RESULT"/>
+    <tableColumn id="10" xr3:uid="{F64D71F0-DE72-41E5-A09A-AEF089CE68AF}" name="OBSERVATIONS"/>
   </tableColumns>
   <tableStyleInfo name="GE3 2021 F2-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43" headerRowDxfId="1">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="PATH"/>
@@ -1127,187 +1639,187 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1365,19 +1877,19 @@
         <v>4</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>5</v>
@@ -1391,29 +1903,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K2" s="2">
         <v>923412921</v>
@@ -1422,10 +1934,10 @@
         <v>45</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1439,23 +1951,23 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K3" s="2">
         <v>923412921</v>
@@ -1464,10 +1976,10 @@
         <v>45</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1481,23 +1993,23 @@
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K4" s="2">
         <v>923412921</v>
@@ -1506,14 +2018,14 @@
         <v>45</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1523,23 +2035,23 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H5" s="14">
         <v>99999</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K5" s="2">
         <v>923412921</v>
@@ -1548,10 +2060,10 @@
         <v>45</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="O5" s="24"/>
     </row>
@@ -1560,29 +2072,29 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K6" s="2">
         <v>666111222</v>
@@ -1591,10 +2103,10 @@
         <v>12</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1602,29 +2114,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K7" s="2">
         <v>552555222</v>
@@ -1633,10 +2145,10 @@
         <v>56</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1650,23 +2162,23 @@
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K8" s="2">
         <v>923412341</v>
@@ -1675,10 +2187,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N8" s="23" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1692,23 +2204,23 @@
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I9" s="13">
         <v>234231</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K9" s="2">
         <v>923412341</v>
@@ -1717,10 +2229,10 @@
         <v>8</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1734,23 +2246,23 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="K10" s="2">
         <v>923412921</v>
@@ -1759,10 +2271,10 @@
         <v>45</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N10" s="23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1776,23 +2288,23 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K11" s="2">
         <v>923412921</v>
@@ -1801,10 +2313,10 @@
         <v>45</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N11" s="23" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1818,23 +2330,23 @@
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K12" s="2">
         <v>923412921</v>
@@ -1843,10 +2355,10 @@
         <v>45</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1860,23 +2372,23 @@
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K13" s="13">
         <v>99123</v>
@@ -1885,10 +2397,10 @@
         <v>45</v>
       </c>
       <c r="M13" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1902,23 +2414,23 @@
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K14" s="13">
         <v>23424534324</v>
@@ -1927,10 +2439,10 @@
         <v>45</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1944,35 +2456,35 @@
         <v>8</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L15" s="2">
         <v>45</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1986,23 +2498,23 @@
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="K16" s="17">
         <v>685838390</v>
@@ -2011,10 +2523,10 @@
         <v>5</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N16" s="23" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2028,23 +2540,23 @@
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K17" s="17">
         <v>685838390</v>
@@ -2053,10 +2565,10 @@
         <v>126</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2070,35 +2582,35 @@
         <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="I18" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="K18" s="17">
         <v>685838390</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2106,29 +2618,29 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="K19" s="2">
         <v>678923456</v>
@@ -2137,10 +2649,10 @@
         <v>34</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2148,29 +2660,29 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
@@ -2179,10 +2691,10 @@
         <v>6</v>
       </c>
       <c r="M20" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2190,29 +2702,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K21" s="2">
         <v>918234765</v>
@@ -2221,10 +2733,10 @@
         <v>125</v>
       </c>
       <c r="M21" s="22" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N21" s="23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2232,29 +2744,29 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K22" s="1">
         <v>925902123</v>
@@ -2263,10 +2775,10 @@
         <v>89</v>
       </c>
       <c r="M22" s="23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N22" s="23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2274,29 +2786,29 @@
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K23" s="1">
         <v>925902123</v>
@@ -2305,10 +2817,10 @@
         <v>89</v>
       </c>
       <c r="M23" s="23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3304,8 +3816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3322,31 +3834,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="8" t="s">
@@ -3354,495 +3866,1107 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="B6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="B9" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="B10" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+      <c r="B16" s="1">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
+      <c r="B21" s="1">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+      <c r="B22" s="1">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="B23" s="1">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
+      <c r="B24" s="1">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="B25" s="1">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
+      <c r="B26" s="1">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="B27" s="1">
+        <v>16</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
+      <c r="B28" s="1">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="B29" s="1">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="B30" s="1">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="B38" s="1">
+        <v>22.35</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4871,7 +5995,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3</v>
@@ -4880,7 +6004,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>5</v>
@@ -4894,11 +6018,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -4911,7 +6035,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4924,7 +6048,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4937,7 +6061,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -4950,7 +6074,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4961,7 +6085,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4972,7 +6096,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -4983,7 +6107,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -4994,7 +6118,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -5005,7 +6129,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -5016,7 +6140,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5027,7 +6151,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -5038,7 +6162,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -5049,7 +6173,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -5060,7 +6184,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>

</xml_diff>

<commit_message>
Añadidos tests para el requisito 2
</commit_message>
<xml_diff>
--- a/docs/Casos de prueba.xlsx
+++ b/docs/Casos de prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\PycharmProjects\G80.2022.T10.EG3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F03CA4F-A75E-485C-B479-97527D3B22E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7CA5AC-C531-4BE6-A406-A9D84CA97C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="2352" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="6" r:id="rId1"/>
@@ -1129,7 +1129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1163,6 +1163,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,7 +1398,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C943CFE-479E-4F17-9794-3B0A241BDC37}" name="Table_32" displayName="Table_32" ref="A1:J43" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C943CFE-479E-4F17-9794-3B0A241BDC37}" name="Table_32" displayName="Table_32" ref="A1:J43" headerRowDxfId="1">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{93B13E22-E985-4930-A193-EA9B9D4B2027}" name="#"/>
     <tableColumn id="2" xr3:uid="{BE1F42EC-89F3-4ED3-A311-BA3B85140EF4}" name="NODE"/>
@@ -1413,7 +1416,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43" headerRowDxfId="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="PATH"/>
@@ -1831,7 +1834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3816,8 +3819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3828,7 +3831,7 @@
     <col min="5" max="5" width="22.1796875" customWidth="1"/>
     <col min="6" max="6" width="62.1796875" customWidth="1"/>
     <col min="7" max="7" width="9.1796875" customWidth="1"/>
-    <col min="8" max="8" width="36.81640625" customWidth="1"/>
+    <col min="8" max="8" width="66.26953125" customWidth="1"/>
     <col min="9" max="10" width="33.81640625" customWidth="1"/>
     <col min="11" max="28" width="10.54296875" customWidth="1"/>
   </cols>
@@ -4057,7 +4060,7 @@
       <c r="E8" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="28" t="s">
         <v>171</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -4085,7 +4088,7 @@
       <c r="E9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="28" t="s">
         <v>175</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -4113,7 +4116,7 @@
       <c r="E10" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="28" t="s">
         <v>180</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -4141,7 +4144,7 @@
       <c r="E11" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="28" t="s">
         <v>184</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -4169,7 +4172,7 @@
       <c r="E12" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="28" t="s">
         <v>188</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -4197,7 +4200,7 @@
       <c r="E13" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="28" t="s">
         <v>192</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -4225,7 +4228,7 @@
       <c r="E14" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="28" t="s">
         <v>196</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -4253,7 +4256,7 @@
       <c r="E15" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="28" t="s">
         <v>200</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -4281,7 +4284,7 @@
       <c r="E16" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="28" t="s">
         <v>204</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -4309,7 +4312,7 @@
       <c r="E17" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="28" t="s">
         <v>208</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -4337,7 +4340,7 @@
       <c r="E18" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="28" t="s">
         <v>212</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -4365,7 +4368,7 @@
       <c r="E19" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="28" t="s">
         <v>217</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -4393,7 +4396,7 @@
       <c r="E20" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="28" t="s">
         <v>221</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -4421,7 +4424,7 @@
       <c r="E21" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="28" t="s">
         <v>225</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -4449,7 +4452,7 @@
       <c r="E22" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="28" t="s">
         <v>229</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -4477,7 +4480,7 @@
       <c r="E23" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="29" t="s">
         <v>233</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -4505,7 +4508,7 @@
       <c r="E24" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="28" t="s">
         <v>237</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -4533,7 +4536,7 @@
       <c r="E25" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="28" t="s">
         <v>241</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -4561,7 +4564,7 @@
       <c r="E26" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="28" t="s">
         <v>245</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -4589,7 +4592,7 @@
       <c r="E27" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="28" t="s">
         <v>249</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -4617,7 +4620,7 @@
       <c r="E28" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="28" t="s">
         <v>253</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -4645,7 +4648,7 @@
       <c r="E29" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="28" t="s">
         <v>257</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -4673,7 +4676,7 @@
       <c r="E30" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="28" t="s">
         <v>261</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -4701,7 +4704,7 @@
       <c r="E31" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="28" t="s">
         <v>266</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -4731,7 +4734,7 @@
       <c r="E32" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="28" t="s">
         <v>272</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -4759,7 +4762,7 @@
       <c r="E33" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="28" t="s">
         <v>276</v>
       </c>
       <c r="G33" s="1" t="s">
@@ -4787,7 +4790,7 @@
       <c r="E34" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="28" t="s">
         <v>281</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -4974,7 +4977,7 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="E41" s="27"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -5964,9 +5967,9 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Añadidos tests de modificaciones. Editados los tests de get_vaccine_date para hacer todos los incorrectos en uno.
</commit_message>
<xml_diff>
--- a/docs/Casos de prueba.xlsx
+++ b/docs/Casos de prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamy\PycharmProjects\G80.2022.T10.EG3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CE882C-597E-40E1-A394-CAB61412613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327D5261-6CCB-42E3-BF08-92AD82ED4B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="410">
   <si>
     <t>I/O</t>
   </si>
@@ -1113,6 +1113,198 @@
   </si>
   <si>
     <t>22, 35</t>
+  </si>
+  <si>
+    <t>MODIFICATION</t>
+  </si>
+  <si>
+    <t>test_corchete1modificado</t>
+  </si>
+  <si>
+    <t>El primer corchete es una 'a'.</t>
+  </si>
+  <si>
+    <t>test_corchete1modificado.json</t>
+  </si>
+  <si>
+    <t>a"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_corchete2modificado</t>
+  </si>
+  <si>
+    <t>El segundo corchete es 77</t>
+  </si>
+  <si>
+    <t>test_corchete2modificado.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"77</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>test_comamodificada</t>
+  </si>
+  <si>
+    <t>La coma es una c</t>
+  </si>
+  <si>
+    <t>test_comamodificada.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93"c"ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_igualdad1modificada</t>
+  </si>
+  <si>
+    <t>La primera igualdad es una g</t>
+  </si>
+  <si>
+    <t>test_igualdad1modificada.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID"g"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_igualdad2modificada</t>
+  </si>
+  <si>
+    <t>La segunda igualdad es un guion (-)</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber"-"923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla1modificada</t>
+  </si>
+  <si>
+    <t>La primera comilla es 10</t>
+  </si>
+  <si>
+    <t>{10PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla2modificada</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID7:"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>La segunda comilla es 7</t>
+  </si>
+  <si>
+    <t>test_comilla3modificada</t>
+  </si>
+  <si>
+    <t>La tercera comilla es 7</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":71c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla4modificada</t>
+  </si>
+  <si>
+    <t>La cuarta comilla es 'a'</t>
+  </si>
+  <si>
+    <t>test_comilla4modificada.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93a,"ContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla5modificada</t>
+  </si>
+  <si>
+    <t>La quinta comilla es 'a'</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93",aContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla6modificada</t>
+  </si>
+  <si>
+    <t>test_test_comilla6modificada.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumberm:"923412921"}</t>
+  </si>
+  <si>
+    <t>La sexta comilla es 'm'</t>
+  </si>
+  <si>
+    <t>test_comilla7modificada</t>
+  </si>
+  <si>
+    <t>La séptima comilla es 'numero'</t>
+  </si>
+  <si>
+    <t>test_test_comilla7modificada.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":numero923412921"}</t>
+  </si>
+  <si>
+    <t>test_comilla8modificada</t>
+  </si>
+  <si>
+    <t>test_test_comilla8modificada.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":"923412921a}</t>
+  </si>
+  <si>
+    <t>La octava comilla es 'a'</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta1modificado</t>
+  </si>
+  <si>
+    <t>PatientSystemID' es 'ID'</t>
+  </si>
+  <si>
+    <t>{"ID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta1modificado.json</t>
+  </si>
+  <si>
+    <t>test_valordato1modificado</t>
+  </si>
+  <si>
+    <t>Valor de 'PatientSystemID' es 3</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"3","ContactPhoneNumber":"923412921"}</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta2modificado</t>
+  </si>
+  <si>
+    <t>ContactPhoneNumber' es a</t>
+  </si>
+  <si>
+    <t>test_valoretiqueta2modificado.json</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","a": "923412921"}</t>
+  </si>
+  <si>
+    <t>test_valordato2modificado</t>
+  </si>
+  <si>
+    <t>valor de 'ContactPhoneNumber' es ?</t>
+  </si>
+  <si>
+    <t>{"PatientSystemID":"1c3349220ec3a91d8848c03e5d272d93","ContactPhoneNumber": "?"}</t>
+  </si>
+  <si>
+    <t>test_valordato2modificado.json</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1272,6 +1464,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,7 +1697,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C943CFE-479E-4F17-9794-3B0A241BDC37}" name="Table_32" displayName="Table_32" ref="A1:J49" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C943CFE-479E-4F17-9794-3B0A241BDC37}" name="Table_32" displayName="Table_32" ref="A1:J65" headerRowDxfId="1">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{93B13E22-E985-4930-A193-EA9B9D4B2027}" name="#"/>
     <tableColumn id="2" xr3:uid="{BE1F42EC-89F3-4ED3-A311-BA3B85140EF4}" name="NODE"/>
@@ -1522,7 +1715,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_4" displayName="Table_4" ref="A1:G43" headerRowDxfId="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="PATH"/>
@@ -3925,8 +4118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.15234375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5304,47 +5497,481 @@
     </row>
     <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="1"/>
+      <c r="B49" s="1">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="H49" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1">
+        <v>9</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1">
+        <v>13</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H52" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1">
+        <v>27</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1">
+        <v>31</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1">
+        <v>33</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1">
+        <v>34</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1">
+        <v>36</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1">
+        <v>37</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H58" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1">
+        <v>39</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="H59" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1">
+        <v>40</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H60" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1">
+        <v>42</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H61" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1">
+        <v>32</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F62" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H62" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1">
+        <v>35</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="F63" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="H63" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1">
+        <v>38</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="H64" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1">
+        <v>41</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>407</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H65" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Tests de request_vaccine_manager modificados para reflejar valores límite, requirements y Excel actualizados
</commit_message>
<xml_diff>
--- a/docs/Casos de prueba.xlsx
+++ b/docs/Casos de prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamy\PycharmProjects\G80.2022.T10.EG3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327D5261-6CCB-42E3-BF08-92AD82ED4B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13563AE5-F3E3-4C1F-849E-B2EE021F2FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="411">
   <si>
     <t>I/O</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Toby Woof</t>
   </si>
   <si>
-    <t>José Federicogonzaloramonperecianorodríguez</t>
-  </si>
-  <si>
     <t>Feliciano</t>
   </si>
   <si>
@@ -389,15 +386,9 @@
     <t>Esternilocideo Masterianosones</t>
   </si>
   <si>
-    <t>Pruebo valor de 30 caracteres para nombre y edad mínima (6)</t>
-  </si>
-  <si>
     <t>C J</t>
   </si>
   <si>
-    <t>Pruebo valor máximo de edad y nombre corto</t>
-  </si>
-  <si>
     <t>INPUT/OUTPUT</t>
   </si>
   <si>
@@ -428,27 +419,15 @@
     <t>Registration type incorrecto</t>
   </si>
   <si>
-    <t>Nombre que excede 30 caracteres</t>
-  </si>
-  <si>
     <t>Formato de nombre incorrecto</t>
   </si>
   <si>
     <t>Formato de nombre incorrecto (muchas palabras)</t>
   </si>
   <si>
-    <t>Teléfono demasiado largo</t>
-  </si>
-  <si>
     <t>Teléfono con formato incorrecto</t>
   </si>
   <si>
-    <t>Edad muy baja</t>
-  </si>
-  <si>
-    <t>Edad que supera el máximo</t>
-  </si>
-  <si>
     <t>Formato de edad incorrecto</t>
   </si>
   <si>
@@ -488,9 +467,6 @@
     <t>"31e68fe8-13dd-4dd3-9b81-69a66cb80a91"</t>
   </si>
   <si>
-    <t>Teléfono demasiado corto</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -1305,6 +1281,33 @@
   </si>
   <si>
     <t>test_valordato2modificado.json</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>Edad muy baja (Valor límite)</t>
+  </si>
+  <si>
+    <t>Edad que supera el máximo (Valor límite)</t>
+  </si>
+  <si>
+    <t>Teléfono demasiado corto (Valor límite)</t>
+  </si>
+  <si>
+    <t>Teléfono demasiado largo (Valor límite)</t>
+  </si>
+  <si>
+    <t>Pruebo valor de 30 caracteres (valor límite) para nombre y edad mínima (6, valor límite)</t>
+  </si>
+  <si>
+    <t>Pruebo valor máximo de edad y nombre corto (valor límite de nombre)</t>
+  </si>
+  <si>
+    <t>UnNombreDeMas TreintaCaracteres</t>
+  </si>
+  <si>
+    <t>Nombre de 31 caracteres (valor límite)</t>
   </si>
 </sst>
 </file>
@@ -1675,8 +1678,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:N23" headerRowDxfId="5">
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A1:O23" headerRowDxfId="5">
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="#"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="I/O"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TECHNIQUE"/>
@@ -1691,6 +1694,7 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="age"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="EXPECTED RESULT" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="OBSERVATIONS" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B47BB01F-5F35-4891-9AA2-271CBCCB3D5A}" name="Columna1"/>
   </tableColumns>
   <tableStyleInfo name="GE3 2021 F1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1930,7 +1934,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1974,7 +1978,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>40</v>
@@ -1982,7 +1986,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>41</v>
@@ -1990,10 +1994,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2017,7 +2021,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2033,7 +2037,7 @@
         <v>57</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2041,7 +2045,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2049,15 +2053,15 @@
         <v>59</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2065,15 +2069,15 @@
         <v>61</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -2081,12 +2085,12 @@
         <v>62</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>51</v>
@@ -2094,7 +2098,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>52</v>
@@ -2105,7 +2109,7 @@
         <v>63</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -2113,7 +2117,7 @@
         <v>64</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -2121,7 +2125,7 @@
         <v>65</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2133,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.15234375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2152,8 +2156,9 @@
     <col min="11" max="11" width="13.4609375" customWidth="1"/>
     <col min="12" max="12" width="9.4609375" customWidth="1"/>
     <col min="13" max="13" width="29.84375" customWidth="1"/>
-    <col min="14" max="14" width="51" customWidth="1"/>
-    <col min="15" max="32" width="10.53515625" customWidth="1"/>
+    <col min="14" max="14" width="67.07421875" customWidth="1"/>
+    <col min="15" max="15" width="22.84375" customWidth="1"/>
+    <col min="16" max="32" width="10.53515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2199,26 +2204,29 @@
       <c r="N1" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="O1" s="9" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>67</v>
@@ -2239,7 +2247,7 @@
         <v>28</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2281,7 +2289,7 @@
         <v>29</v>
       </c>
       <c r="N3" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2323,7 +2331,7 @@
         <v>29</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2365,7 +2373,7 @@
         <v>29</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="O5" s="24"/>
     </row>
@@ -2374,20 +2382,20 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>71</v>
@@ -2396,7 +2404,7 @@
         <v>70</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6" s="2">
         <v>666111222</v>
@@ -2408,7 +2416,7 @@
         <v>28</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2416,20 +2424,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>73</v>
@@ -2450,7 +2458,7 @@
         <v>28</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2471,13 +2479,13 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>67</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>74</v>
@@ -2492,7 +2500,7 @@
         <v>29</v>
       </c>
       <c r="N8" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2513,7 +2521,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>67</v>
@@ -2534,7 +2542,7 @@
         <v>29</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2548,7 +2556,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>12</v>
@@ -2564,7 +2572,7 @@
         <v>30</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>75</v>
+        <v>409</v>
       </c>
       <c r="K10" s="2">
         <v>923412921</v>
@@ -2576,7 +2584,7 @@
         <v>29</v>
       </c>
       <c r="N10" s="23" t="s">
-        <v>117</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2590,7 +2598,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>12</v>
@@ -2606,7 +2614,7 @@
         <v>30</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K11" s="2">
         <v>923412921</v>
@@ -2618,7 +2626,7 @@
         <v>29</v>
       </c>
       <c r="N11" s="23" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2632,7 +2640,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>12</v>
@@ -2648,7 +2656,7 @@
         <v>30</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K12" s="2">
         <v>923412921</v>
@@ -2660,7 +2668,7 @@
         <v>29</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2693,7 +2701,7 @@
         <v>66</v>
       </c>
       <c r="K13" s="13">
-        <v>99123</v>
+        <v>12345678</v>
       </c>
       <c r="L13" s="2">
         <v>45</v>
@@ -2702,7 +2710,7 @@
         <v>29</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>137</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2735,7 +2743,7 @@
         <v>66</v>
       </c>
       <c r="K14" s="13">
-        <v>23424534324</v>
+        <v>9123456789</v>
       </c>
       <c r="L14" s="2">
         <v>45</v>
@@ -2744,7 +2752,7 @@
         <v>29</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>120</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2777,7 +2785,7 @@
         <v>66</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L15" s="2">
         <v>45</v>
@@ -2786,7 +2794,7 @@
         <v>29</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2828,7 +2836,7 @@
         <v>29</v>
       </c>
       <c r="N16" s="23" t="s">
-        <v>122</v>
+        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2849,7 +2857,7 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>67</v>
@@ -2870,7 +2878,7 @@
         <v>29</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>123</v>
+        <v>404</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2906,13 +2914,13 @@
         <v>685838390</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M18" s="22" t="s">
         <v>29</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2920,29 +2928,29 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K19" s="2">
         <v>678923456</v>
@@ -2954,7 +2962,7 @@
         <v>28</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2962,29 +2970,29 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>70</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
@@ -2996,7 +3004,7 @@
         <v>28</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>104</v>
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3004,29 +3012,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K21" s="2">
         <v>918234765</v>
@@ -3038,7 +3046,7 @@
         <v>28</v>
       </c>
       <c r="N21" s="23" t="s">
-        <v>106</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3046,13 +3054,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>11</v>
@@ -3062,13 +3070,13 @@
         <v>65</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="K22" s="1">
         <v>925902123</v>
@@ -3077,10 +3085,10 @@
         <v>89</v>
       </c>
       <c r="M22" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" s="23" t="s">
         <v>99</v>
-      </c>
-      <c r="N22" s="23" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -3088,13 +3096,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>12</v>
@@ -3104,13 +3112,13 @@
         <v>64</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>30</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K23" s="1">
         <v>925902123</v>
@@ -3122,7 +3130,7 @@
         <v>29</v>
       </c>
       <c r="N23" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4118,8 +4126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.15234375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4172,28 +4180,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="J2" s="25"/>
     </row>
@@ -4205,22 +4213,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>29</v>
@@ -4235,22 +4243,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>29</v>
@@ -4265,22 +4273,22 @@
         <v>2.5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>29</v>
@@ -4295,22 +4303,22 @@
         <v>2.5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>29</v>
@@ -4323,22 +4331,22 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>29</v>
@@ -4351,22 +4359,22 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>29</v>
@@ -4379,22 +4387,22 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>29</v>
@@ -4407,22 +4415,22 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>29</v>
@@ -4435,22 +4443,22 @@
         <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>29</v>
@@ -4463,22 +4471,22 @@
         <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>29</v>
@@ -4491,22 +4499,22 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>29</v>
@@ -4519,22 +4527,22 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>29</v>
@@ -4547,22 +4555,22 @@
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>29</v>
@@ -4575,22 +4583,22 @@
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>29</v>
@@ -4603,22 +4611,22 @@
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>29</v>
@@ -4631,22 +4639,22 @@
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>29</v>
@@ -4656,25 +4664,25 @@
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>29</v>
@@ -4684,25 +4692,25 @@
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>29</v>
@@ -4715,22 +4723,22 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>29</v>
@@ -4743,22 +4751,22 @@
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>29</v>
@@ -4771,22 +4779,22 @@
         <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>29</v>
@@ -4799,22 +4807,22 @@
         <v>14</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>29</v>
@@ -4827,22 +4835,22 @@
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>29</v>
@@ -4855,22 +4863,22 @@
         <v>15</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>29</v>
@@ -4883,22 +4891,22 @@
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="F27" s="27" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>29</v>
@@ -4911,22 +4919,22 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F28" s="27" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>29</v>
@@ -4939,22 +4947,22 @@
         <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>29</v>
@@ -4967,22 +4975,22 @@
         <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>29</v>
@@ -4992,55 +5000,55 @@
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>29</v>
@@ -5050,25 +5058,25 @@
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>29</v>
@@ -5078,25 +5086,25 @@
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>29</v>
@@ -5106,25 +5114,25 @@
     <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>29</v>
@@ -5134,25 +5142,25 @@
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>29</v>
@@ -5162,25 +5170,25 @@
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>29</v>
@@ -5190,25 +5198,25 @@
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>29</v>
@@ -5218,25 +5226,25 @@
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="H39" s="1" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>29</v>
@@ -5246,25 +5254,25 @@
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>29</v>
@@ -5274,25 +5282,25 @@
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>29</v>
@@ -5302,25 +5310,25 @@
     <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>29</v>
@@ -5330,25 +5338,25 @@
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>29</v>
@@ -5358,25 +5366,25 @@
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="H44" s="26" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>29</v>
@@ -5386,25 +5394,25 @@
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H45" s="26" t="s">
         <v>322</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="H45" s="26" t="s">
-        <v>330</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>29</v>
@@ -5414,25 +5422,25 @@
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>29</v>
@@ -5442,25 +5450,25 @@
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H47" s="26" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>29</v>
@@ -5470,25 +5478,25 @@
     <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H48" s="26" t="s">
         <v>336</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="H48" s="26" t="s">
-        <v>344</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>29</v>
@@ -5501,22 +5509,22 @@
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>29</v>
@@ -5529,22 +5537,22 @@
         <v>9</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H50" s="26" t="s">
         <v>346</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>354</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>29</v>
@@ -5557,22 +5565,22 @@
         <v>13</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>29</v>
@@ -5585,22 +5593,22 @@
         <v>20</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H52" s="26" t="s">
         <v>355</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="H52" s="26" t="s">
-        <v>363</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>29</v>
@@ -5612,22 +5620,22 @@
         <v>27</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>29</v>
@@ -5639,22 +5647,22 @@
         <v>31</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>29</v>
@@ -5666,22 +5674,22 @@
         <v>33</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>29</v>
@@ -5693,22 +5701,22 @@
         <v>34</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>29</v>
@@ -5720,22 +5728,22 @@
         <v>36</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>29</v>
@@ -5747,22 +5755,22 @@
         <v>37</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>29</v>
@@ -5774,22 +5782,22 @@
         <v>39</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>29</v>
@@ -5801,22 +5809,22 @@
         <v>40</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>29</v>
@@ -5828,22 +5836,22 @@
         <v>42</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>29</v>
@@ -5855,22 +5863,22 @@
         <v>32</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="F62" s="29" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>29</v>
@@ -5882,22 +5890,22 @@
         <v>35</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="F63" s="29" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>29</v>
@@ -5909,22 +5917,22 @@
         <v>38</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="F64" s="29" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>29</v>
@@ -5936,22 +5944,22 @@
         <v>41</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="F65" s="29" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>29</v>

</xml_diff>